<commit_message>
Chnage in utility fn
Added work dummy in utility function and recalibrated the associated parameter
</commit_message>
<xml_diff>
--- a/data/labor_choice.xlsx
+++ b/data/labor_choice.xlsx
@@ -412,13 +412,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.653232397092348</v>
       </c>
       <c r="D3">
         <v>0.6489827483892441</v>
       </c>
       <c r="E3">
-        <v>2.9244079271595E-05</v>
+        <v>2.9244079271595e-05</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -426,13 +426,13 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.7087294077164609</v>
+        <v>0.494567508279926</v>
       </c>
       <c r="D4">
         <v>0.646990367770195</v>
       </c>
       <c r="E4">
-        <v>2.731052891648926E-05</v>
+        <v>2.731052891648926e-05</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -440,13 +440,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>-0.105699478094628</v>
+        <v>-0.1970354481462937</v>
       </c>
       <c r="D5">
         <v>-0.0005530303256819025</v>
       </c>
       <c r="E5">
-        <v>7.88234048219924E-05</v>
+        <v>7.88234048219924e-05</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -454,10 +454,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>-0.22964324383684</v>
       </c>
       <c r="D6">
-        <v>-0.3254977791559269</v>
+        <v>-0.3254977791559274</v>
       </c>
       <c r="E6">
         <v>0.03794091047325767</v>
@@ -468,13 +468,13 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.08201177580355344</v>
       </c>
       <c r="D7">
         <v>0.1167982742482005</v>
       </c>
       <c r="E7">
-        <v>0.002933956643042228</v>
+        <v>0.002933956643042229</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -482,13 +482,13 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.1776880348197343</v>
       </c>
       <c r="D8">
         <v>0.2522709802401231</v>
       </c>
       <c r="E8">
-        <v>6.191117344771943E-05</v>
+        <v>6.191117344771939e-05</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -496,13 +496,13 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.007251142640212443</v>
+        <v>0.008220003613187324</v>
       </c>
       <c r="D9">
-        <v>0.161154425275725</v>
+        <v>0.1611544252757249</v>
       </c>
       <c r="E9">
-        <v>0.02682390016553198</v>
+        <v>0.02682390016553195</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -510,10 +510,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>5.18784086007588E-07</v>
+        <v>0.0001622621681291687</v>
       </c>
       <c r="D10">
-        <v>-0.003200531431248728</v>
+        <v>-0.003200531431248727</v>
       </c>
       <c r="E10">
         <v>0.001356443954006627</v>
@@ -524,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>-0.005741201080244453</v>
+        <v>-0.005741201080244457</v>
       </c>
       <c r="D11">
         <v>-0.00580307850426516</v>
@@ -538,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1.356604303901077</v>
+        <v>1.440248505367899</v>
       </c>
       <c r="D12">
         <v>1.003455477952957</v>

</xml_diff>

<commit_message>
Included sigma2 of non-earned income
Included variance of shocks in the process of non-earned income
</commit_message>
<xml_diff>
--- a/data/labor_choice.xlsx
+++ b/data/labor_choice.xlsx
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.6459331584154158</v>
+        <v>0.8191621144995483</v>
       </c>
       <c r="D3">
         <v>0.6477891474962234</v>
@@ -426,7 +426,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.5686932771301991</v>
+        <v>0.5990300658092822</v>
       </c>
       <c r="D4">
         <v>0.6474272519350052</v>
@@ -440,7 +440,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>-0.004762919091807542</v>
+        <v>-0.05884812859031883</v>
       </c>
       <c r="D5">
         <v>0.004535745471366681</v>
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>-0.1969974170554449</v>
+        <v>-0.2477909811474888</v>
       </c>
       <c r="D6">
         <v>-0.3330443065773845</v>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.07028126911280778</v>
+        <v>0.08798946409716052</v>
       </c>
       <c r="D7">
         <v>0.1174455500094394</v>
@@ -482,7 +482,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.1523710074302076</v>
+        <v>0.1903335571888334</v>
       </c>
       <c r="D8">
         <v>0.2505834270102912</v>
@@ -496,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.1856900061531385</v>
+        <v>0.08731620729673588</v>
       </c>
       <c r="D9">
         <v>0.1532139450442513</v>
@@ -510,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>-0.000160400273378614</v>
+        <v>-0.0001454401703124805</v>
       </c>
       <c r="D10">
         <v>-0.003125279552280412</v>
@@ -538,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1.440100937578702</v>
+        <v>1.386943624147526</v>
       </c>
       <c r="D12">
         <v>0.9952412724494935</v>

</xml_diff>

<commit_message>
Fixed bootstrap and incluided W matrix
Fixed SE calculation in the variance-cov matrix of moments.
Defined W matrix as the inverse of the diagonal matrices of variances
</commit_message>
<xml_diff>
--- a/data/labor_choice.xlsx
+++ b/data/labor_choice.xlsx
@@ -412,13 +412,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.8191621144995483</v>
+        <v>0.6750737666136178</v>
       </c>
       <c r="D3">
         <v>0.6477891474962234</v>
       </c>
       <c r="E3">
-        <v>1.987539742889733e-05</v>
+        <v>0.003030525623108707</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -426,13 +426,13 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.5990300658092822</v>
+        <v>0.6363529614176954</v>
       </c>
       <c r="D4">
         <v>0.6474272519350052</v>
       </c>
       <c r="E4">
-        <v>1.679572380768059e-05</v>
+        <v>0.002560948606935951</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -440,13 +440,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>-0.05884812859031883</v>
+        <v>0.1097145765582836</v>
       </c>
       <c r="D5">
         <v>0.004535745471366681</v>
       </c>
       <c r="E5">
-        <v>8.255132463054791e-05</v>
+        <v>0.01258711456761647</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -454,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>-0.2477909811474888</v>
+        <v>-0.2507780460882012</v>
       </c>
       <c r="D6">
         <v>-0.3330443065773845</v>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.08798946409716052</v>
+        <v>0.0961140756678302</v>
       </c>
       <c r="D7">
         <v>0.1174455500094394</v>
@@ -482,13 +482,13 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.1903335571888334</v>
+        <v>0.1627879618544771</v>
       </c>
       <c r="D8">
         <v>0.2505834270102912</v>
       </c>
       <c r="E8">
-        <v>5.168099690416847e-05</v>
+        <v>0.007880123449414392</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -496,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.08731620729673588</v>
+        <v>0.2529853398853936</v>
       </c>
       <c r="D9">
         <v>0.1532139450442513</v>
@@ -510,7 +510,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>-0.0001454401703124805</v>
+        <v>-7.968197710167701e-06</v>
       </c>
       <c r="D10">
         <v>-0.003125279552280412</v>
@@ -524,7 +524,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>-0.005741201080244457</v>
+        <v>-0.005741201080244458</v>
       </c>
       <c r="D11">
         <v>-0.0055716239958156</v>
@@ -538,13 +538,13 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>1.386943624147526</v>
+        <v>1.524337807788891</v>
       </c>
       <c r="D12">
         <v>0.9952412724494935</v>
       </c>
       <c r="E12">
-        <v>0.0001067675603138048</v>
+        <v>0.01627951483261187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>